<commit_message>
chore: update setup-repo pages
</commit_message>
<xml_diff>
--- a/setup-repo/CodeSystem-mii-cs-fall-supplement-act-encounter-code.xlsx
+++ b/setup-repo/CodeSystem-mii-cs-fall-supplement-act-encounter-code.xlsx
@@ -30,7 +30,7 @@
     <t>Version</t>
   </si>
   <si>
-    <t>2026.0.0-dev.1</t>
+    <t>2026.0.0</t>
   </si>
   <si>
     <t>Name</t>
@@ -60,7 +60,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2025-12-03T10:23:08+00:00</t>
+    <t>2025-12-11T17:49:30+00:00</t>
   </si>
   <si>
     <t>Publisher</t>

</xml_diff>